<commit_message>
Update Test cases for Tip calculator.xlsx
</commit_message>
<xml_diff>
--- a/Tip Calculator/Test cases for Tip calculator.xlsx
+++ b/Tip Calculator/Test cases for Tip calculator.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="178">
   <si>
     <t>Project Name:</t>
   </si>
@@ -187,6 +187,34 @@
     <t>TC_08</t>
   </si>
   <si>
+    <t>Verify that error appears when invalid value entered in bill</t>
+  </si>
+  <si>
+    <t>1. Launch the application
+2. Enter the invalid values</t>
+  </si>
+  <si>
+    <t>"test"</t>
+  </si>
+  <si>
+    <t>error message should pop-up</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>Verify that error appears when invalid value entered in Tip %</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>Verify that error appears when invalid value entered in  Number of People</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
     <t>Verify that error message pops up when calculate is clicked without entering any values</t>
   </si>
   <si>
@@ -197,7 +225,7 @@
     <t>error message should pop up when calculate is clicked without entering any values</t>
   </si>
   <si>
-    <t>TC_09</t>
+    <t>TC_12</t>
   </si>
   <si>
     <t>Verify that error message pops up when only one input field is entered</t>
@@ -211,7 +239,7 @@
     <t xml:space="preserve">error message should pop up </t>
   </si>
   <si>
-    <t>TC_10</t>
+    <t>TC_13</t>
   </si>
   <si>
     <t>Verify that tips is calculated when all input fields are filled</t>
@@ -225,7 +253,7 @@
     <t>tips is calculated</t>
   </si>
   <si>
-    <t>TC_11</t>
+    <t>TC_14</t>
   </si>
   <si>
     <t>Verify that "Tip per person" and "Total per person" shows up when valid values are entered</t>
@@ -239,7 +267,7 @@
     <t>"Tip per person" and "Total per person" should show up when valid values are entered</t>
   </si>
   <si>
-    <t>TC_12</t>
+    <t>TC_15</t>
   </si>
   <si>
     <t>Verify that "Tip per person" and "Total per person" doesnt show up when invalid values are entered</t>
@@ -253,7 +281,7 @@
     <t>"Tip per person" and "Total per person" shouldnt show up when invalid values are entered</t>
   </si>
   <si>
-    <t>TC_13</t>
+    <t>TC_16</t>
   </si>
   <si>
     <t>Verify that "Tip per person" and "Total per person" values contains '$' sign</t>
@@ -268,7 +296,7 @@
     <t>Tip per person" and "Total per person" values should contain '$' sign</t>
   </si>
   <si>
-    <t>TC_14</t>
+    <t>TC_17</t>
   </si>
   <si>
     <t>Verify that "Tip per person" and "Total per person" values are upto two decimal points</t>
@@ -283,7 +311,7 @@
     <t>"Tip per person" and "Total per person" values should be upto two decimal points</t>
   </si>
   <si>
-    <t>TC_15</t>
+    <t>TC_18</t>
   </si>
   <si>
     <t>Verify that error message appears when "Number of people" value entered is 0</t>
@@ -297,7 +325,7 @@
     <t>error message should appear when "Number of people" value entered is 0</t>
   </si>
   <si>
-    <t>TC_16</t>
+    <t>TC_19</t>
   </si>
   <si>
     <t>Verify that error message appears when user enters negative numbers in any input</t>
@@ -311,7 +339,7 @@
     <t>error message should appear when user enters negative numbers in any input</t>
   </si>
   <si>
-    <t>TC_17</t>
+    <t>TC_20</t>
   </si>
   <si>
     <t>Verify that step indicator is present in input</t>
@@ -325,7 +353,7 @@
     <t>step indicator should be present in input</t>
   </si>
   <si>
-    <t>TC_18</t>
+    <t>TC_21</t>
   </si>
   <si>
     <t>Verify that "down arrow" decreases the input value</t>
@@ -339,7 +367,7 @@
     <t>"down arrow" should decrease the input value</t>
   </si>
   <si>
-    <t>TC_19</t>
+    <t>TC_22</t>
   </si>
   <si>
     <t>Verify that "up arrow" increases the input value</t>
@@ -353,7 +381,7 @@
     <t>"up arrow" should increase the input value</t>
   </si>
   <si>
-    <t>TC_20</t>
+    <t>TC_23</t>
   </si>
   <si>
     <t>Verify that number intervals for "Bill" is 0.01</t>
@@ -370,7 +398,7 @@
     <t>number intervals for "Bill" should be 0.01</t>
   </si>
   <si>
-    <t>TC_21</t>
+    <t>TC_24</t>
   </si>
   <si>
     <t>Verify that number intervals for "Tip %" is 1</t>
@@ -384,7 +412,7 @@
     <t>number intervals for "Tip %" should be 1</t>
   </si>
   <si>
-    <t>TC_22</t>
+    <t>TC_25</t>
   </si>
   <si>
     <t>Verify that number intervals for "Number of People" is 1</t>
@@ -398,7 +426,7 @@
     <t>number intervals for "Number of People" should be 1</t>
   </si>
   <si>
-    <t>TC_23</t>
+    <t>TC_26</t>
   </si>
   <si>
     <t>Verify that minimum value for Bill is 0 in step indicator</t>
@@ -412,7 +440,7 @@
     <t>minimum value for Bill should be 0</t>
   </si>
   <si>
-    <t>TC_24</t>
+    <t>TC_27</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that minimum value for Tip% is 0 in step indicator </t>
@@ -426,7 +454,7 @@
     <t>minimum value for Tip% should be 0</t>
   </si>
   <si>
-    <t>TC_25</t>
+    <t>TC_28</t>
   </si>
   <si>
     <t>Verify that minimum value for Number of People is 1 in step indicator</t>
@@ -440,7 +468,7 @@
     <t>minimum value for Number of People should be 1</t>
   </si>
   <si>
-    <t>TC_26</t>
+    <t>TC_29</t>
   </si>
   <si>
     <t>Verify that decimal number input in "Tip%"is converted to natural number</t>
@@ -461,7 +489,7 @@
     <t>Tip%" should get converted to natural number</t>
   </si>
   <si>
-    <t>TC_27</t>
+    <t>TC_30</t>
   </si>
   <si>
     <t>Verify that decimal number input in "Number of People" is converted to natural number</t>
@@ -479,7 +507,7 @@
     <t>"Number of People" should get converted to natural number</t>
   </si>
   <si>
-    <t>TC_28</t>
+    <t>TC_31</t>
   </si>
   <si>
     <t>Verify that input "Bill" only takes number upto two decimal places</t>
@@ -497,7 +525,7 @@
     <t>"Bill" should only takes number upto two decimal places</t>
   </si>
   <si>
-    <t>TC_29</t>
+    <t>TC_32</t>
   </si>
   <si>
     <t>Verify that user is able to delete the input one by one with backspace key</t>
@@ -511,7 +539,7 @@
     <t>user should be able to delete the input one by one with backspace key</t>
   </si>
   <si>
-    <t>TC_30</t>
+    <t>TC_33</t>
   </si>
   <si>
     <t>Verify that user is able to delete the input one by one with delete key</t>
@@ -526,7 +554,7 @@
     <t>user should be able to delete the input one by one with delete key</t>
   </si>
   <si>
-    <t>TC_31</t>
+    <t>TC_34</t>
   </si>
   <si>
     <t>Verify that Tip is calculated when "enter" key is pressed inside Bill input</t>
@@ -541,7 +569,7 @@
     <t>Tip should be calculated when "enter" key is pressed</t>
   </si>
   <si>
-    <t>TC_32</t>
+    <t>TC_35</t>
   </si>
   <si>
     <t>Verify that Tip is calculated when "enter" key is pressed inside Tip % input</t>
@@ -553,7 +581,7 @@
 4. press enter key</t>
   </si>
   <si>
-    <t>TC_33</t>
+    <t>TC_36</t>
   </si>
   <si>
     <t>Verify that Tip is calculated when "enter" key is pressed inside  Number of People input</t>
@@ -565,7 +593,7 @@
 4. press enter key</t>
   </si>
   <si>
-    <t>TC_34</t>
+    <t>TC_37</t>
   </si>
   <si>
     <t>Verify that Tip is not calculated when "enter" key is pressed outside the input</t>
@@ -580,7 +608,7 @@
     <t>Tip should not be calculated when "enter" key is pressed</t>
   </si>
   <si>
-    <t>TC_35</t>
+    <t>TC_38</t>
   </si>
   <si>
     <t>Verify that Tip is not calculated when "enter" key is hold</t>
@@ -1168,7 +1196,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="12">
-        <v>44437.0</v>
+        <v>44438.0</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1429,701 +1457,760 @@
       <c r="C17" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="25"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="G17" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="26"/>
     </row>
     <row r="18">
       <c r="A18" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="26"/>
+        <v>55</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="G18" s="24" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="26"/>
+        <v>55</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="G19" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>64</v>
+        <v>30</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
     </row>
     <row r="20">
       <c r="A20" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="30"/>
+      <c r="C20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="25"/>
       <c r="E20" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="26"/>
+        <v>64</v>
+      </c>
       <c r="G20" s="24" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="26"/>
     </row>
     <row r="21">
       <c r="A21" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="30"/>
+      <c r="C21" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F21" s="26"/>
       <c r="G21" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="25"/>
+        <v>71</v>
+      </c>
+      <c r="D22" s="28"/>
       <c r="E22" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F22" s="26"/>
       <c r="G22" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="26"/>
     </row>
     <row r="23">
       <c r="A23" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
     </row>
     <row r="24">
       <c r="A24" s="24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="25"/>
+      <c r="C24" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="30"/>
       <c r="E24" s="25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I24" s="26"/>
       <c r="J24" s="26"/>
     </row>
     <row r="25">
       <c r="A25" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="24" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
     </row>
     <row r="26">
       <c r="A26" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="25"/>
+      <c r="C26" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="30"/>
       <c r="E26" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F26" s="26"/>
       <c r="G26" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
     </row>
     <row r="27">
       <c r="A27" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F27" s="26"/>
       <c r="G27" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I27" s="26"/>
       <c r="J27" s="26"/>
     </row>
     <row r="28">
       <c r="A28" s="24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F28" s="26"/>
       <c r="G28" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I28" s="26"/>
       <c r="J28" s="26"/>
     </row>
     <row r="29">
       <c r="A29" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="24" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I29" s="26"/>
       <c r="J29" s="26"/>
     </row>
     <row r="30">
       <c r="A30" s="24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F30" s="26"/>
       <c r="G30" s="24" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
     </row>
     <row r="31">
       <c r="A31" s="24" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F31" s="26"/>
       <c r="G31" s="24" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I31" s="26"/>
       <c r="J31" s="26"/>
     </row>
     <row r="32">
       <c r="A32" s="24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="24" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
     </row>
     <row r="33">
       <c r="A33" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F33" s="26"/>
       <c r="G33" s="24" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="H33" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
     </row>
     <row r="34">
       <c r="A34" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="24" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I34" s="26"/>
       <c r="J34" s="26"/>
     </row>
     <row r="35">
       <c r="A35" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>128</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>130</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="F35" s="26"/>
       <c r="G35" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I35" s="26"/>
       <c r="J35" s="26"/>
     </row>
     <row r="36">
       <c r="A36" s="24" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="25" t="s">
         <v>128</v>
       </c>
+      <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>135</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F36" s="26"/>
       <c r="G36" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H36" s="27" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I36" s="26"/>
       <c r="J36" s="26"/>
     </row>
     <row r="37">
       <c r="A37" s="24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>128</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>140</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F37" s="26"/>
       <c r="G37" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H37" s="27" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I37" s="26"/>
       <c r="J37" s="26"/>
     </row>
     <row r="38">
       <c r="A38" s="24" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="D38" s="25"/>
+        <v>136</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="E38" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" s="26"/>
+        <v>138</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>139</v>
+      </c>
       <c r="G38" s="24" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H38" s="27" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
     </row>
     <row r="39">
       <c r="A39" s="24" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="25"/>
+        <v>142</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="E39" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="F39" s="26"/>
+        <v>143</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>144</v>
+      </c>
       <c r="G39" s="24" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I39" s="26"/>
       <c r="J39" s="26"/>
     </row>
     <row r="40">
       <c r="A40" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D40" s="31"/>
+        <v>147</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="E40" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="F40" s="26"/>
+        <v>148</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>149</v>
+      </c>
       <c r="G40" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H40" s="27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I40" s="26"/>
       <c r="J40" s="26"/>
     </row>
     <row r="41">
       <c r="A41" s="24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="31"/>
+        <v>152</v>
+      </c>
+      <c r="D41" s="25"/>
       <c r="E41" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F41" s="26"/>
       <c r="G41" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H41" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I41" s="26"/>
       <c r="J41" s="26"/>
     </row>
     <row r="42">
       <c r="A42" s="24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="D42" s="31"/>
+        <v>156</v>
+      </c>
+      <c r="D42" s="25"/>
       <c r="E42" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H42" s="27" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
     </row>
     <row r="43">
       <c r="A43" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" s="31"/>
       <c r="E43" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F43" s="26"/>
       <c r="G43" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I43" s="26"/>
       <c r="J43" s="26"/>
     </row>
     <row r="44">
       <c r="A44" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C44" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="31"/>
+      <c r="E44" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="D44" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>167</v>
-      </c>
+      <c r="F44" s="26"/>
       <c r="G44" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H44" s="25" t="s">
-        <v>168</v>
+        <v>30</v>
+      </c>
+      <c r="H44" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="I44" s="26"/>
       <c r="J44" s="26"/>
     </row>
     <row r="45">
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="H45" s="33"/>
+      <c r="A45" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" s="31"/>
+      <c r="E45" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="F45" s="26"/>
+      <c r="G45" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46">
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="H46" s="33"/>
+      <c r="A46" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="31"/>
+      <c r="E46" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="F46" s="26"/>
+      <c r="G46" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47">
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="H47" s="33"/>
+      <c r="A47" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48">
       <c r="C48" s="32"/>
@@ -7860,6 +7947,24 @@
       <c r="D1003" s="32"/>
       <c r="E1003" s="32"/>
       <c r="H1003" s="33"/>
+    </row>
+    <row r="1004">
+      <c r="C1004" s="32"/>
+      <c r="D1004" s="32"/>
+      <c r="E1004" s="32"/>
+      <c r="H1004" s="33"/>
+    </row>
+    <row r="1005">
+      <c r="C1005" s="32"/>
+      <c r="D1005" s="32"/>
+      <c r="E1005" s="32"/>
+      <c r="H1005" s="33"/>
+    </row>
+    <row r="1006">
+      <c r="C1006" s="32"/>
+      <c r="D1006" s="32"/>
+      <c r="E1006" s="32"/>
+      <c r="H1006" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>